<commit_message>
Add 'Riemann Zeta Function' folder, refactor
</commit_message>
<xml_diff>
--- a/Ruby/Julia Sets/julia.xlsx
+++ b/Ruby/Julia Sets/julia.xlsx
@@ -633,11 +633,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="196303872"/>
-        <c:axId val="196317952"/>
+        <c:axId val="195976192"/>
+        <c:axId val="195986176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="196303872"/>
+        <c:axId val="195976192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,12 +661,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196317952"/>
+        <c:crossAx val="195986176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196317952"/>
+        <c:axId val="195986176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,7 +697,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196303872"/>
+        <c:crossAx val="195976192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -818,11 +818,11 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.44278</cdr:x>
+      <cdr:x>0.41402</cdr:x>
       <cdr:y>0.01989</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.59497</cdr:x>
+      <cdr:x>0.60516</cdr:x>
       <cdr:y>0.0756</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -832,8 +832,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5631180" y="114278"/>
-          <a:ext cx="1935464" cy="320080"/>
+          <a:off x="5265421" y="114278"/>
+          <a:ext cx="2430818" cy="320080"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -1303,7 +1303,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A91:B3146"/>
+  <dimension ref="A91:B5760"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1339,26 +1339,41 @@
     <row r="1440" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B1440" s="1"/>
     </row>
-    <row r="1728" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B1728" s="1"/>
-    </row>
-    <row r="1947" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B1947" s="1"/>
-    </row>
-    <row r="2154" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2154" s="1"/>
-    </row>
-    <row r="2244" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2244" s="1"/>
-    </row>
-    <row r="2335" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2335" s="1"/>
-    </row>
-    <row r="2453" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2453" s="1"/>
-    </row>
-    <row r="3146" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3146" s="1"/>
+    <row r="1800" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B1800" s="1"/>
+    </row>
+    <row r="2160" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2160" s="1"/>
+    </row>
+    <row r="2520" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2520" s="1"/>
+    </row>
+    <row r="2880" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2880" s="1"/>
+    </row>
+    <row r="3240" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3240" s="1"/>
+    </row>
+    <row r="3600" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3600" s="1"/>
+    </row>
+    <row r="3960" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3960" s="1"/>
+    </row>
+    <row r="4320" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4320" s="1"/>
+    </row>
+    <row r="4680" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4680" s="1"/>
+    </row>
+    <row r="5040" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5040" s="1"/>
+    </row>
+    <row r="5400" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5400" s="1"/>
+    </row>
+    <row r="5760" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B5760" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>